<commit_message>
Minor changes to manuscript
Removed metadata table from manuscript, moved it together w/ raw qPCR spreadsheet.
</commit_message>
<xml_diff>
--- a/210621 - AG thesis/Raw/Metadata/Metadata_NESTP.xlsx
+++ b/210621 - AG thesis/Raw/Metadata/Metadata_NESTP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TL\Work\Research\Dr. Uyaguari\AG\AG-TL-MUD-human-enteric-viruses-quantitation\210621 - AG thesis\Raw\Metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ED53191-7F74-4EB1-86B3-A4B661A4CF7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36CFEA65-9DF6-4CF6-A506-7D94C661AA11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -655,7 +655,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="32">
+  <borders count="31">
     <border>
       <left/>
       <right/>
@@ -1007,25 +1007,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="189">
+  <cellXfs count="188">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
@@ -1425,6 +1412,114 @@
     <xf numFmtId="0" fontId="18" fillId="11" borderId="30" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="9" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="30" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="9" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="9" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="9" fillId="12" borderId="30" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="5" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="5" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="5" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1524,134 +1619,25 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="1" fontId="7" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="5" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="2" fontId="7" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="2" fontId="7" fillId="5" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="5" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="30" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="30" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="9" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="30" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="9" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="9" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="9" fillId="12" borderId="30" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3666,77 +3652,77 @@
   <sheetData>
     <row r="1" spans="1:75" s="2" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1"/>
-      <c r="B1" s="131" t="s">
+      <c r="B1" s="160" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="132"/>
-      <c r="D1" s="132"/>
-      <c r="E1" s="132"/>
-      <c r="F1" s="132"/>
-      <c r="G1" s="132"/>
-      <c r="H1" s="133"/>
-      <c r="I1" s="134" t="s">
+      <c r="C1" s="161"/>
+      <c r="D1" s="161"/>
+      <c r="E1" s="161"/>
+      <c r="F1" s="161"/>
+      <c r="G1" s="161"/>
+      <c r="H1" s="162"/>
+      <c r="I1" s="163" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="135"/>
-      <c r="K1" s="135"/>
-      <c r="L1" s="135"/>
-      <c r="M1" s="135"/>
-      <c r="N1" s="136"/>
-      <c r="O1" s="137" t="s">
+      <c r="J1" s="164"/>
+      <c r="K1" s="164"/>
+      <c r="L1" s="164"/>
+      <c r="M1" s="164"/>
+      <c r="N1" s="165"/>
+      <c r="O1" s="166" t="s">
         <v>2</v>
       </c>
-      <c r="P1" s="138"/>
-      <c r="Q1" s="138"/>
-      <c r="R1" s="138"/>
-      <c r="S1" s="138"/>
-      <c r="T1" s="138"/>
-      <c r="U1" s="138"/>
-      <c r="V1" s="138"/>
-      <c r="W1" s="138"/>
-      <c r="X1" s="138"/>
-      <c r="Y1" s="138"/>
-      <c r="Z1" s="138"/>
-      <c r="AA1" s="138"/>
-      <c r="AB1" s="138"/>
-      <c r="AC1" s="138"/>
-      <c r="AD1" s="138"/>
-      <c r="AE1" s="138"/>
-      <c r="AF1" s="139"/>
-      <c r="AG1" s="140"/>
-      <c r="AH1" s="141"/>
-      <c r="AI1" s="141"/>
-      <c r="AJ1" s="141"/>
-      <c r="AK1" s="141"/>
-      <c r="AL1" s="141"/>
-      <c r="AM1" s="141"/>
-      <c r="AN1" s="141"/>
-      <c r="AO1" s="141"/>
-      <c r="AP1" s="141"/>
-      <c r="AQ1" s="141"/>
-      <c r="AR1" s="141"/>
-      <c r="AS1" s="141"/>
-      <c r="AT1" s="141"/>
-      <c r="AU1" s="141"/>
-      <c r="AV1" s="141"/>
-      <c r="AW1" s="141"/>
-      <c r="AX1" s="141"/>
-      <c r="AY1" s="141"/>
-      <c r="AZ1" s="141"/>
-      <c r="BA1" s="141"/>
-      <c r="BB1" s="141"/>
-      <c r="BC1" s="141"/>
-      <c r="BD1" s="141"/>
-      <c r="BE1" s="141"/>
-      <c r="BF1" s="142"/>
-      <c r="BP1" s="128" t="s">
+      <c r="P1" s="167"/>
+      <c r="Q1" s="167"/>
+      <c r="R1" s="167"/>
+      <c r="S1" s="167"/>
+      <c r="T1" s="167"/>
+      <c r="U1" s="167"/>
+      <c r="V1" s="167"/>
+      <c r="W1" s="167"/>
+      <c r="X1" s="167"/>
+      <c r="Y1" s="167"/>
+      <c r="Z1" s="167"/>
+      <c r="AA1" s="167"/>
+      <c r="AB1" s="167"/>
+      <c r="AC1" s="167"/>
+      <c r="AD1" s="167"/>
+      <c r="AE1" s="167"/>
+      <c r="AF1" s="168"/>
+      <c r="AG1" s="169"/>
+      <c r="AH1" s="170"/>
+      <c r="AI1" s="170"/>
+      <c r="AJ1" s="170"/>
+      <c r="AK1" s="170"/>
+      <c r="AL1" s="170"/>
+      <c r="AM1" s="170"/>
+      <c r="AN1" s="170"/>
+      <c r="AO1" s="170"/>
+      <c r="AP1" s="170"/>
+      <c r="AQ1" s="170"/>
+      <c r="AR1" s="170"/>
+      <c r="AS1" s="170"/>
+      <c r="AT1" s="170"/>
+      <c r="AU1" s="170"/>
+      <c r="AV1" s="170"/>
+      <c r="AW1" s="170"/>
+      <c r="AX1" s="170"/>
+      <c r="AY1" s="170"/>
+      <c r="AZ1" s="170"/>
+      <c r="BA1" s="170"/>
+      <c r="BB1" s="170"/>
+      <c r="BC1" s="170"/>
+      <c r="BD1" s="170"/>
+      <c r="BE1" s="170"/>
+      <c r="BF1" s="171"/>
+      <c r="BP1" s="157" t="s">
         <v>3</v>
       </c>
-      <c r="BQ1" s="128"/>
-      <c r="BR1" s="128" t="s">
+      <c r="BQ1" s="157"/>
+      <c r="BR1" s="157" t="s">
         <v>4</v>
       </c>
-      <c r="BS1" s="128"/>
+      <c r="BS1" s="157"/>
       <c r="BT1" s="3"/>
       <c r="BU1" s="3"/>
       <c r="BV1" s="3"/>
@@ -3744,109 +3730,109 @@
     </row>
     <row r="2" spans="1:75" s="5" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4"/>
-      <c r="B2" s="143" t="s">
+      <c r="B2" s="172" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="144"/>
-      <c r="D2" s="145"/>
-      <c r="E2" s="146" t="s">
+      <c r="C2" s="173"/>
+      <c r="D2" s="174"/>
+      <c r="E2" s="175" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="143" t="s">
+      <c r="F2" s="172" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="145"/>
-      <c r="H2" s="148" t="s">
+      <c r="G2" s="174"/>
+      <c r="H2" s="177" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="150" t="s">
+      <c r="I2" s="179" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="151"/>
-      <c r="K2" s="151"/>
-      <c r="L2" s="151"/>
-      <c r="M2" s="152"/>
-      <c r="N2" s="129" t="s">
+      <c r="J2" s="180"/>
+      <c r="K2" s="180"/>
+      <c r="L2" s="180"/>
+      <c r="M2" s="181"/>
+      <c r="N2" s="158" t="s">
         <v>10</v>
       </c>
-      <c r="O2" s="155" t="s">
+      <c r="O2" s="182" t="s">
         <v>11</v>
       </c>
-      <c r="P2" s="156"/>
-      <c r="Q2" s="157"/>
-      <c r="R2" s="158" t="s">
+      <c r="P2" s="152"/>
+      <c r="Q2" s="183"/>
+      <c r="R2" s="151" t="s">
         <v>12</v>
       </c>
-      <c r="S2" s="156"/>
-      <c r="T2" s="157"/>
-      <c r="U2" s="158" t="s">
+      <c r="S2" s="152"/>
+      <c r="T2" s="183"/>
+      <c r="U2" s="151" t="s">
         <v>13</v>
       </c>
-      <c r="V2" s="156"/>
-      <c r="W2" s="157"/>
-      <c r="X2" s="158" t="s">
+      <c r="V2" s="152"/>
+      <c r="W2" s="183"/>
+      <c r="X2" s="151" t="s">
         <v>14</v>
       </c>
-      <c r="Y2" s="156"/>
-      <c r="Z2" s="156"/>
-      <c r="AA2" s="156"/>
-      <c r="AB2" s="156"/>
-      <c r="AC2" s="159"/>
-      <c r="AD2" s="160" t="s">
+      <c r="Y2" s="152"/>
+      <c r="Z2" s="152"/>
+      <c r="AA2" s="152"/>
+      <c r="AB2" s="152"/>
+      <c r="AC2" s="153"/>
+      <c r="AD2" s="154" t="s">
         <v>15</v>
       </c>
-      <c r="AE2" s="161"/>
-      <c r="AF2" s="162"/>
-      <c r="AG2" s="163" t="s">
+      <c r="AE2" s="155"/>
+      <c r="AF2" s="156"/>
+      <c r="AG2" s="140" t="s">
         <v>16</v>
       </c>
-      <c r="AH2" s="164"/>
-      <c r="AI2" s="165"/>
-      <c r="AJ2" s="166" t="s">
+      <c r="AH2" s="141"/>
+      <c r="AI2" s="144"/>
+      <c r="AJ2" s="143" t="s">
         <v>17</v>
       </c>
-      <c r="AK2" s="164"/>
-      <c r="AL2" s="165"/>
-      <c r="AM2" s="164" t="s">
+      <c r="AK2" s="141"/>
+      <c r="AL2" s="144"/>
+      <c r="AM2" s="141" t="s">
         <v>18</v>
       </c>
-      <c r="AN2" s="164"/>
-      <c r="AO2" s="164"/>
-      <c r="AP2" s="166" t="s">
+      <c r="AN2" s="141"/>
+      <c r="AO2" s="141"/>
+      <c r="AP2" s="143" t="s">
         <v>19</v>
       </c>
-      <c r="AQ2" s="164"/>
-      <c r="AR2" s="165"/>
-      <c r="AS2" s="164" t="s">
+      <c r="AQ2" s="141"/>
+      <c r="AR2" s="144"/>
+      <c r="AS2" s="141" t="s">
         <v>20</v>
       </c>
-      <c r="AT2" s="164"/>
-      <c r="AU2" s="164"/>
-      <c r="AV2" s="172" t="s">
+      <c r="AT2" s="141"/>
+      <c r="AU2" s="141"/>
+      <c r="AV2" s="145" t="s">
         <v>21</v>
       </c>
-      <c r="AW2" s="153" t="s">
+      <c r="AW2" s="147" t="s">
         <v>22</v>
       </c>
-      <c r="AX2" s="153" t="s">
+      <c r="AX2" s="147" t="s">
         <v>23</v>
       </c>
-      <c r="AY2" s="174" t="s">
+      <c r="AY2" s="149" t="s">
         <v>24</v>
       </c>
-      <c r="AZ2" s="167" t="s">
+      <c r="AZ2" s="136" t="s">
         <v>25</v>
       </c>
-      <c r="BA2" s="169" t="s">
+      <c r="BA2" s="138" t="s">
         <v>26</v>
       </c>
-      <c r="BB2" s="163" t="s">
+      <c r="BB2" s="140" t="s">
         <v>27</v>
       </c>
-      <c r="BC2" s="164"/>
-      <c r="BD2" s="164"/>
-      <c r="BE2" s="164"/>
-      <c r="BF2" s="171"/>
+      <c r="BC2" s="141"/>
+      <c r="BD2" s="141"/>
+      <c r="BE2" s="141"/>
+      <c r="BF2" s="142"/>
       <c r="BP2" s="6"/>
       <c r="BQ2" s="6"/>
       <c r="BR2" s="6"/>
@@ -3869,14 +3855,14 @@
       <c r="D3" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="E3" s="147"/>
+      <c r="E3" s="176"/>
       <c r="F3" s="11" t="s">
         <v>32</v>
       </c>
       <c r="G3" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="H3" s="149"/>
+      <c r="H3" s="178"/>
       <c r="I3" s="13" t="s">
         <v>34</v>
       </c>
@@ -3892,7 +3878,7 @@
       <c r="M3" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="N3" s="130"/>
+      <c r="N3" s="159"/>
       <c r="O3" s="16" t="s">
         <v>34</v>
       </c>
@@ -3992,12 +3978,12 @@
       <c r="AU3" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="AV3" s="173"/>
-      <c r="AW3" s="154"/>
-      <c r="AX3" s="154"/>
-      <c r="AY3" s="175"/>
-      <c r="AZ3" s="168"/>
-      <c r="BA3" s="170"/>
+      <c r="AV3" s="146"/>
+      <c r="AW3" s="148"/>
+      <c r="AX3" s="148"/>
+      <c r="AY3" s="150"/>
+      <c r="AZ3" s="137"/>
+      <c r="BA3" s="139"/>
       <c r="BB3" s="34" t="s">
         <v>10</v>
       </c>
@@ -6380,19 +6366,6 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="AZ2:AZ3"/>
-    <mergeCell ref="BA2:BA3"/>
-    <mergeCell ref="BB2:BF2"/>
-    <mergeCell ref="AP2:AR2"/>
-    <mergeCell ref="AS2:AU2"/>
-    <mergeCell ref="AV2:AV3"/>
-    <mergeCell ref="AX2:AX3"/>
-    <mergeCell ref="AY2:AY3"/>
-    <mergeCell ref="X2:AC2"/>
-    <mergeCell ref="AD2:AF2"/>
-    <mergeCell ref="AG2:AI2"/>
-    <mergeCell ref="AJ2:AL2"/>
-    <mergeCell ref="AM2:AO2"/>
     <mergeCell ref="BP1:BQ1"/>
     <mergeCell ref="BR1:BS1"/>
     <mergeCell ref="N2:N3"/>
@@ -6409,6 +6382,19 @@
     <mergeCell ref="O2:Q2"/>
     <mergeCell ref="R2:T2"/>
     <mergeCell ref="U2:W2"/>
+    <mergeCell ref="X2:AC2"/>
+    <mergeCell ref="AD2:AF2"/>
+    <mergeCell ref="AG2:AI2"/>
+    <mergeCell ref="AJ2:AL2"/>
+    <mergeCell ref="AM2:AO2"/>
+    <mergeCell ref="AZ2:AZ3"/>
+    <mergeCell ref="BA2:BA3"/>
+    <mergeCell ref="BB2:BF2"/>
+    <mergeCell ref="AP2:AR2"/>
+    <mergeCell ref="AS2:AU2"/>
+    <mergeCell ref="AV2:AV3"/>
+    <mergeCell ref="AX2:AX3"/>
+    <mergeCell ref="AY2:AY3"/>
   </mergeCells>
   <conditionalFormatting sqref="A1:A3">
     <cfRule type="expression" dxfId="119" priority="125">
@@ -8585,8 +8571,8 @@
   <dimension ref="A1:X54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="X17" sqref="X17"/>
+      <pane xSplit="2" topLeftCell="J1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="O20" sqref="O20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8597,33 +8583,30 @@
     <col min="4" max="4" width="11.33203125" customWidth="1"/>
     <col min="5" max="5" width="10.33203125" customWidth="1"/>
     <col min="6" max="6" width="15.6640625" customWidth="1"/>
-    <col min="7" max="7" width="11.109375" customWidth="1"/>
-    <col min="8" max="8" width="11.77734375" customWidth="1"/>
-    <col min="9" max="9" width="12.88671875" customWidth="1"/>
-    <col min="10" max="10" width="12.33203125" customWidth="1"/>
-    <col min="11" max="11" width="11.5546875" customWidth="1"/>
-    <col min="12" max="12" width="12.6640625" customWidth="1"/>
+    <col min="7" max="7" width="10.88671875" customWidth="1"/>
+    <col min="8" max="12" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13.33203125" customWidth="1"/>
-    <col min="14" max="14" width="12.88671875" customWidth="1"/>
-    <col min="15" max="15" width="11.88671875" customWidth="1"/>
-    <col min="16" max="16" width="12" customWidth="1"/>
-    <col min="17" max="17" width="11.44140625" customWidth="1"/>
-    <col min="18" max="18" width="13.77734375" customWidth="1"/>
-    <col min="19" max="19" width="20.88671875" customWidth="1"/>
+    <col min="14" max="14" width="13" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.77734375" customWidth="1"/>
+    <col min="19" max="19" width="22.33203125" customWidth="1"/>
     <col min="20" max="20" width="13.77734375" customWidth="1"/>
     <col min="21" max="21" width="13.77734375" style="112" customWidth="1"/>
     <col min="22" max="22" width="13.77734375" customWidth="1"/>
-    <col min="23" max="24" width="21.109375" customWidth="1"/>
+    <col min="23" max="23" width="21.109375" customWidth="1"/>
+    <col min="24" max="24" width="22.77734375" customWidth="1"/>
     <col min="25" max="25" width="30" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="21.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:24" ht="84.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G1" s="176" t="s">
+      <c r="G1" s="184" t="s">
         <v>99</v>
       </c>
-      <c r="H1" s="176"/>
-      <c r="I1" s="176"/>
+      <c r="H1" s="184"/>
+      <c r="I1" s="184"/>
     </row>
     <row r="3" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B3" s="81" t="s">
@@ -9558,384 +9541,384 @@
       <c r="U16" s="116"/>
       <c r="V16" s="88"/>
     </row>
-    <row r="17" spans="1:24" s="177" customFormat="1" ht="40.200000000000003" x14ac:dyDescent="0.3">
-      <c r="A17" s="186" t="s">
+    <row r="17" spans="1:24" s="128" customFormat="1" ht="40.200000000000003" x14ac:dyDescent="0.3">
+      <c r="A17" s="185" t="s">
         <v>100</v>
       </c>
-      <c r="B17" s="186" t="s">
+      <c r="B17" s="185" t="s">
         <v>101</v>
       </c>
-      <c r="C17" s="187" t="s">
+      <c r="C17" s="186" t="s">
         <v>62</v>
       </c>
-      <c r="D17" s="187" t="s">
+      <c r="D17" s="186" t="s">
         <v>51</v>
       </c>
-      <c r="E17" s="187" t="s">
+      <c r="E17" s="186" t="s">
         <v>102</v>
       </c>
-      <c r="F17" s="187" t="s">
+      <c r="F17" s="186" t="s">
         <v>64</v>
       </c>
-      <c r="G17" s="187" t="s">
+      <c r="G17" s="186" t="s">
         <v>52</v>
       </c>
-      <c r="H17" s="187" t="s">
+      <c r="H17" s="186" t="s">
         <v>65</v>
       </c>
-      <c r="I17" s="187" t="s">
+      <c r="I17" s="186" t="s">
         <v>66</v>
       </c>
-      <c r="J17" s="187" t="s">
+      <c r="J17" s="186" t="s">
         <v>55</v>
       </c>
-      <c r="K17" s="187" t="s">
+      <c r="K17" s="186" t="s">
         <v>54</v>
       </c>
-      <c r="L17" s="187" t="s">
+      <c r="L17" s="186" t="s">
         <v>56</v>
       </c>
-      <c r="M17" s="187" t="s">
+      <c r="M17" s="186" t="s">
         <v>57</v>
       </c>
-      <c r="N17" s="187" t="s">
+      <c r="N17" s="186" t="s">
         <v>58</v>
       </c>
-      <c r="O17" s="187" t="s">
+      <c r="O17" s="186" t="s">
         <v>59</v>
       </c>
-      <c r="P17" s="187" t="s">
+      <c r="P17" s="186" t="s">
         <v>60</v>
       </c>
-      <c r="Q17" s="187" t="s">
+      <c r="Q17" s="186" t="s">
         <v>61</v>
       </c>
-      <c r="R17" s="187" t="s">
+      <c r="R17" s="186" t="s">
         <v>67</v>
       </c>
-      <c r="S17" s="187" t="s">
+      <c r="S17" s="186" t="s">
         <v>109</v>
       </c>
-      <c r="T17" s="187" t="s">
+      <c r="T17" s="186" t="s">
         <v>69</v>
       </c>
-      <c r="U17" s="187" t="s">
+      <c r="U17" s="186" t="s">
         <v>97</v>
       </c>
-      <c r="V17" s="187" t="s">
+      <c r="V17" s="186" t="s">
         <v>98</v>
       </c>
       <c r="W17" s="127" t="s">
         <v>106</v>
       </c>
-      <c r="X17" s="188" t="s">
+      <c r="X17" s="186" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="18" spans="1:24" s="94" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="178">
+      <c r="A18" s="129">
         <v>1</v>
       </c>
       <c r="B18" s="120">
         <v>43760</v>
       </c>
-      <c r="C18" s="179">
+      <c r="C18" s="130">
         <v>341.37900000000002</v>
       </c>
-      <c r="D18" s="179">
+      <c r="D18" s="130">
         <v>1065</v>
       </c>
-      <c r="E18" s="180">
+      <c r="E18" s="131">
         <v>7.12</v>
       </c>
-      <c r="F18" s="181">
+      <c r="F18" s="132">
         <v>12.234999999999999</v>
       </c>
-      <c r="G18" s="181">
+      <c r="G18" s="132">
         <v>10</v>
       </c>
-      <c r="H18" s="181">
+      <c r="H18" s="132">
         <v>9</v>
       </c>
-      <c r="I18" s="181">
+      <c r="I18" s="132">
         <v>4</v>
       </c>
-      <c r="J18" s="182">
+      <c r="J18" s="133">
         <v>25</v>
       </c>
-      <c r="K18" s="181">
+      <c r="K18" s="132">
         <v>51.5</v>
       </c>
-      <c r="L18" s="181">
+      <c r="L18" s="132">
         <v>5.9050000000000002</v>
       </c>
-      <c r="M18" s="181">
+      <c r="M18" s="132">
         <v>7.49</v>
       </c>
-      <c r="N18" s="181">
+      <c r="N18" s="132">
         <v>1.29</v>
       </c>
-      <c r="O18" s="181">
+      <c r="O18" s="132">
         <v>1.9</v>
       </c>
-      <c r="P18" s="181">
+      <c r="P18" s="132">
         <v>19.8</v>
       </c>
-      <c r="Q18" s="181">
+      <c r="Q18" s="132">
         <v>16.899999999999999</v>
       </c>
-      <c r="R18" s="179">
+      <c r="R18" s="130">
         <v>341</v>
       </c>
-      <c r="S18" s="179">
+      <c r="S18" s="130">
         <v>13.4</v>
       </c>
-      <c r="T18" s="179">
+      <c r="T18" s="130">
         <v>56.7</v>
       </c>
-      <c r="U18" s="183">
+      <c r="U18" s="134">
         <f>U5/100</f>
         <v>0.6</v>
       </c>
-      <c r="V18" s="180">
+      <c r="V18" s="131">
         <f>V5/100</f>
         <v>1</v>
       </c>
-      <c r="W18" s="178">
+      <c r="W18" s="129">
         <v>4.5999999999999996</v>
       </c>
-      <c r="X18" s="184">
+      <c r="X18" s="187">
         <f t="shared" ref="X18" si="0">X5+273.15</f>
         <v>275.84999999999997</v>
       </c>
     </row>
     <row r="19" spans="1:24" s="94" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="178">
+      <c r="A19" s="129">
         <v>2</v>
       </c>
       <c r="B19" s="120">
         <v>43797</v>
       </c>
-      <c r="C19" s="179">
+      <c r="C19" s="130">
         <v>158.36500000000001</v>
       </c>
-      <c r="D19" s="182">
+      <c r="D19" s="133">
         <v>886</v>
       </c>
-      <c r="E19" s="180">
+      <c r="E19" s="131">
         <v>6.81</v>
       </c>
-      <c r="F19" s="179">
+      <c r="F19" s="130">
         <v>4.24</v>
       </c>
-      <c r="G19" s="182">
+      <c r="G19" s="133">
         <v>6</v>
       </c>
-      <c r="H19" s="182">
+      <c r="H19" s="133">
         <v>13</v>
       </c>
-      <c r="I19" s="182">
+      <c r="I19" s="133">
         <v>5</v>
       </c>
-      <c r="J19" s="182">
+      <c r="J19" s="133">
         <v>51</v>
       </c>
-      <c r="K19" s="182">
+      <c r="K19" s="133">
         <v>66</v>
       </c>
-      <c r="L19" s="179">
+      <c r="L19" s="130">
         <v>26.3</v>
       </c>
-      <c r="M19" s="179">
+      <c r="M19" s="130">
         <v>5.33</v>
       </c>
-      <c r="N19" s="180">
+      <c r="N19" s="131">
         <v>2.62</v>
       </c>
-      <c r="O19" s="180">
+      <c r="O19" s="131">
         <v>3.4331999999999998</v>
       </c>
-      <c r="P19" s="179">
+      <c r="P19" s="130">
         <v>21.2</v>
       </c>
-      <c r="Q19" s="179">
+      <c r="Q19" s="130">
         <v>40.700000000000003</v>
       </c>
-      <c r="R19" s="179">
+      <c r="R19" s="130">
         <v>119</v>
       </c>
-      <c r="S19" s="179">
+      <c r="S19" s="130">
         <v>14.1</v>
       </c>
-      <c r="T19" s="179">
+      <c r="T19" s="130">
         <v>52.1</v>
       </c>
-      <c r="U19" s="183">
+      <c r="U19" s="134">
         <f>U8/100</f>
         <v>0.6</v>
       </c>
-      <c r="V19" s="180">
+      <c r="V19" s="131">
         <f>V8/100</f>
         <v>0.2</v>
       </c>
-      <c r="W19" s="178">
+      <c r="W19" s="129">
         <v>0</v>
       </c>
-      <c r="X19" s="184">
+      <c r="X19" s="187">
         <f t="shared" ref="X19" si="1">X8+273.15</f>
         <v>266.54999999999995</v>
       </c>
     </row>
     <row r="20" spans="1:24" s="94" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="178">
+      <c r="A20" s="129">
         <v>3</v>
       </c>
       <c r="B20" s="120">
         <v>43817</v>
       </c>
-      <c r="C20" s="179">
+      <c r="C20" s="130">
         <v>141.30600000000001</v>
       </c>
-      <c r="D20" s="182">
+      <c r="D20" s="133">
         <v>818</v>
       </c>
-      <c r="E20" s="180">
+      <c r="E20" s="131">
         <v>6.79</v>
       </c>
-      <c r="F20" s="179">
+      <c r="F20" s="130">
         <v>6.28</v>
       </c>
-      <c r="G20" s="182">
+      <c r="G20" s="133">
         <v>10</v>
       </c>
-      <c r="H20" s="182">
+      <c r="H20" s="133">
         <v>18</v>
       </c>
-      <c r="I20" s="182">
+      <c r="I20" s="133">
         <v>7</v>
       </c>
-      <c r="J20" s="182">
+      <c r="J20" s="133">
         <v>68</v>
       </c>
-      <c r="K20" s="182">
+      <c r="K20" s="133">
         <v>94</v>
       </c>
-      <c r="L20" s="179">
+      <c r="L20" s="130">
         <v>34.299999999999997</v>
       </c>
-      <c r="M20" s="179">
+      <c r="M20" s="130">
         <v>3.28</v>
       </c>
-      <c r="N20" s="180">
+      <c r="N20" s="131">
         <v>1.1599999999999999</v>
       </c>
-      <c r="O20" s="180">
+      <c r="O20" s="131">
         <v>1.6906000000000001</v>
       </c>
-      <c r="P20" s="179">
+      <c r="P20" s="130">
         <v>29.6</v>
       </c>
-      <c r="Q20" s="179">
+      <c r="Q20" s="130">
         <v>49.8</v>
       </c>
-      <c r="R20" s="179">
+      <c r="R20" s="130">
         <v>223</v>
       </c>
-      <c r="S20" s="179">
+      <c r="S20" s="130">
         <v>14.1</v>
       </c>
-      <c r="T20" s="179">
+      <c r="T20" s="130">
         <v>45.8</v>
       </c>
-      <c r="U20" s="183">
+      <c r="U20" s="134">
         <f>U11/100</f>
         <v>0.9</v>
       </c>
-      <c r="V20" s="180">
+      <c r="V20" s="131">
         <f>V11/100</f>
         <v>0.4</v>
       </c>
-      <c r="W20" s="178">
+      <c r="W20" s="129">
         <v>0</v>
       </c>
-      <c r="X20" s="184">
+      <c r="X20" s="187">
         <f t="shared" ref="X20" si="2">X11+273.15</f>
         <v>256.14999999999998</v>
       </c>
     </row>
     <row r="21" spans="1:24" s="94" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="178">
+      <c r="A21" s="129">
         <v>4</v>
       </c>
       <c r="B21" s="120">
         <v>43867</v>
       </c>
-      <c r="C21" s="179">
+      <c r="C21" s="130">
         <v>135.851</v>
       </c>
-      <c r="D21" s="182">
+      <c r="D21" s="133">
         <v>598</v>
       </c>
-      <c r="E21" s="180">
+      <c r="E21" s="131">
         <v>6.99</v>
       </c>
-      <c r="F21" s="179">
+      <c r="F21" s="130">
         <v>9.24</v>
       </c>
-      <c r="G21" s="182">
+      <c r="G21" s="133">
         <v>18</v>
       </c>
-      <c r="H21" s="182">
+      <c r="H21" s="133">
         <v>26</v>
       </c>
-      <c r="I21" s="182">
+      <c r="I21" s="133">
         <v>7</v>
       </c>
-      <c r="J21" s="182">
+      <c r="J21" s="133">
         <v>63</v>
       </c>
-      <c r="K21" s="182">
+      <c r="K21" s="133">
         <v>89</v>
       </c>
-      <c r="L21" s="179">
+      <c r="L21" s="130">
         <v>34.9</v>
       </c>
-      <c r="M21" s="179">
+      <c r="M21" s="130">
         <v>2.0699999999999998</v>
       </c>
-      <c r="N21" s="180">
+      <c r="N21" s="131">
         <v>1.04</v>
       </c>
-      <c r="O21" s="180">
+      <c r="O21" s="131">
         <v>1.6949000000000001</v>
       </c>
-      <c r="P21" s="179">
+      <c r="P21" s="130">
         <v>34.4</v>
       </c>
-      <c r="Q21" s="179">
+      <c r="Q21" s="130">
         <v>50.5</v>
       </c>
-      <c r="R21" s="179">
+      <c r="R21" s="130">
         <v>140</v>
       </c>
-      <c r="S21" s="179">
+      <c r="S21" s="130">
         <v>12.7</v>
       </c>
-      <c r="T21" s="179">
+      <c r="T21" s="130">
         <v>46.9</v>
       </c>
-      <c r="U21" s="183">
+      <c r="U21" s="134">
         <f>U14/100</f>
         <v>10.8</v>
       </c>
-      <c r="V21" s="185">
+      <c r="V21" s="135">
         <f>V14/100</f>
         <v>6.4</v>
       </c>
-      <c r="W21" s="178">
+      <c r="W21" s="129">
         <v>0</v>
       </c>
-      <c r="X21" s="184">
+      <c r="X21" s="187">
         <f t="shared" ref="X21" si="3">X14+273.15</f>
         <v>256.04999999999995</v>
       </c>

</xml_diff>

<commit_message>
Big Friday manuscript update
Lots of edits to manuscript. 2 supplementary figures and 1 supplementary table were generated. Also edits to R scripts & other files.
</commit_message>
<xml_diff>
--- a/210621 - AG thesis/Raw/Metadata/Metadata_NESTP.xlsx
+++ b/210621 - AG thesis/Raw/Metadata/Metadata_NESTP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TL\Work\Research\Dr. Uyaguari\AG\AG-TL-MUD-human-enteric-viruses-quantitation\210621 - AG thesis\Raw\Metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66AD114B-CD95-4C2F-B5D6-88236416F32F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40A1CA13-DCA3-40E4-ACA3-FF8E25B4AC30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12072" yWindow="4680" windowWidth="10824" windowHeight="7500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Operating data" sheetId="1" r:id="rId1"/>
@@ -1012,7 +1012,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="188">
+  <cellXfs count="194">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
@@ -1445,6 +1445,161 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="5" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="1" fontId="7" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
       <protection locked="0"/>
@@ -1461,26 +1616,10 @@
       <alignment horizontal="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="2" fontId="7" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
       <protection locked="0"/>
@@ -1489,14 +1628,6 @@
       <alignment horizontal="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="1" fontId="7" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="5" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="1" fontId="7" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
       <protection locked="0"/>
@@ -1505,139 +1636,24 @@
       <alignment horizontal="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="16" fillId="0" borderId="28" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="16" fillId="0" borderId="28" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="16" fillId="0" borderId="28" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="16" fillId="0" borderId="28" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="28" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3652,77 +3668,77 @@
   <sheetData>
     <row r="1" spans="1:75" s="2" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1"/>
-      <c r="B1" s="163" t="s">
+      <c r="B1" s="142" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="164"/>
-      <c r="D1" s="164"/>
-      <c r="E1" s="164"/>
-      <c r="F1" s="164"/>
-      <c r="G1" s="164"/>
-      <c r="H1" s="165"/>
-      <c r="I1" s="166" t="s">
+      <c r="C1" s="143"/>
+      <c r="D1" s="143"/>
+      <c r="E1" s="143"/>
+      <c r="F1" s="143"/>
+      <c r="G1" s="143"/>
+      <c r="H1" s="144"/>
+      <c r="I1" s="145" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="167"/>
-      <c r="K1" s="167"/>
-      <c r="L1" s="167"/>
-      <c r="M1" s="167"/>
-      <c r="N1" s="168"/>
-      <c r="O1" s="169" t="s">
+      <c r="J1" s="146"/>
+      <c r="K1" s="146"/>
+      <c r="L1" s="146"/>
+      <c r="M1" s="146"/>
+      <c r="N1" s="147"/>
+      <c r="O1" s="148" t="s">
         <v>2</v>
       </c>
-      <c r="P1" s="170"/>
-      <c r="Q1" s="170"/>
-      <c r="R1" s="170"/>
-      <c r="S1" s="170"/>
-      <c r="T1" s="170"/>
-      <c r="U1" s="170"/>
-      <c r="V1" s="170"/>
-      <c r="W1" s="170"/>
-      <c r="X1" s="170"/>
-      <c r="Y1" s="170"/>
-      <c r="Z1" s="170"/>
-      <c r="AA1" s="170"/>
-      <c r="AB1" s="170"/>
-      <c r="AC1" s="170"/>
-      <c r="AD1" s="170"/>
-      <c r="AE1" s="170"/>
-      <c r="AF1" s="171"/>
-      <c r="AG1" s="172"/>
-      <c r="AH1" s="173"/>
-      <c r="AI1" s="173"/>
-      <c r="AJ1" s="173"/>
-      <c r="AK1" s="173"/>
-      <c r="AL1" s="173"/>
-      <c r="AM1" s="173"/>
-      <c r="AN1" s="173"/>
-      <c r="AO1" s="173"/>
-      <c r="AP1" s="173"/>
-      <c r="AQ1" s="173"/>
-      <c r="AR1" s="173"/>
-      <c r="AS1" s="173"/>
-      <c r="AT1" s="173"/>
-      <c r="AU1" s="173"/>
-      <c r="AV1" s="173"/>
-      <c r="AW1" s="173"/>
-      <c r="AX1" s="173"/>
-      <c r="AY1" s="173"/>
-      <c r="AZ1" s="173"/>
-      <c r="BA1" s="173"/>
-      <c r="BB1" s="173"/>
-      <c r="BC1" s="173"/>
-      <c r="BD1" s="173"/>
-      <c r="BE1" s="173"/>
-      <c r="BF1" s="174"/>
-      <c r="BP1" s="160" t="s">
+      <c r="P1" s="149"/>
+      <c r="Q1" s="149"/>
+      <c r="R1" s="149"/>
+      <c r="S1" s="149"/>
+      <c r="T1" s="149"/>
+      <c r="U1" s="149"/>
+      <c r="V1" s="149"/>
+      <c r="W1" s="149"/>
+      <c r="X1" s="149"/>
+      <c r="Y1" s="149"/>
+      <c r="Z1" s="149"/>
+      <c r="AA1" s="149"/>
+      <c r="AB1" s="149"/>
+      <c r="AC1" s="149"/>
+      <c r="AD1" s="149"/>
+      <c r="AE1" s="149"/>
+      <c r="AF1" s="150"/>
+      <c r="AG1" s="151"/>
+      <c r="AH1" s="152"/>
+      <c r="AI1" s="152"/>
+      <c r="AJ1" s="152"/>
+      <c r="AK1" s="152"/>
+      <c r="AL1" s="152"/>
+      <c r="AM1" s="152"/>
+      <c r="AN1" s="152"/>
+      <c r="AO1" s="152"/>
+      <c r="AP1" s="152"/>
+      <c r="AQ1" s="152"/>
+      <c r="AR1" s="152"/>
+      <c r="AS1" s="152"/>
+      <c r="AT1" s="152"/>
+      <c r="AU1" s="152"/>
+      <c r="AV1" s="152"/>
+      <c r="AW1" s="152"/>
+      <c r="AX1" s="152"/>
+      <c r="AY1" s="152"/>
+      <c r="AZ1" s="152"/>
+      <c r="BA1" s="152"/>
+      <c r="BB1" s="152"/>
+      <c r="BC1" s="152"/>
+      <c r="BD1" s="152"/>
+      <c r="BE1" s="152"/>
+      <c r="BF1" s="153"/>
+      <c r="BP1" s="139" t="s">
         <v>3</v>
       </c>
-      <c r="BQ1" s="160"/>
-      <c r="BR1" s="160" t="s">
+      <c r="BQ1" s="139"/>
+      <c r="BR1" s="139" t="s">
         <v>4</v>
       </c>
-      <c r="BS1" s="160"/>
+      <c r="BS1" s="139"/>
       <c r="BT1" s="3"/>
       <c r="BU1" s="3"/>
       <c r="BV1" s="3"/>
@@ -3730,109 +3746,109 @@
     </row>
     <row r="2" spans="1:75" s="5" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4"/>
-      <c r="B2" s="175" t="s">
+      <c r="B2" s="154" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="176"/>
-      <c r="D2" s="177"/>
-      <c r="E2" s="178" t="s">
+      <c r="C2" s="155"/>
+      <c r="D2" s="156"/>
+      <c r="E2" s="157" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="175" t="s">
+      <c r="F2" s="154" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="177"/>
-      <c r="H2" s="180" t="s">
+      <c r="G2" s="156"/>
+      <c r="H2" s="159" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="182" t="s">
+      <c r="I2" s="161" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="183"/>
-      <c r="K2" s="183"/>
-      <c r="L2" s="183"/>
-      <c r="M2" s="184"/>
-      <c r="N2" s="161" t="s">
+      <c r="J2" s="162"/>
+      <c r="K2" s="162"/>
+      <c r="L2" s="162"/>
+      <c r="M2" s="163"/>
+      <c r="N2" s="140" t="s">
         <v>10</v>
       </c>
-      <c r="O2" s="185" t="s">
+      <c r="O2" s="166" t="s">
         <v>11</v>
       </c>
-      <c r="P2" s="155"/>
-      <c r="Q2" s="186"/>
-      <c r="R2" s="154" t="s">
+      <c r="P2" s="167"/>
+      <c r="Q2" s="168"/>
+      <c r="R2" s="169" t="s">
         <v>12</v>
       </c>
-      <c r="S2" s="155"/>
-      <c r="T2" s="186"/>
-      <c r="U2" s="154" t="s">
+      <c r="S2" s="167"/>
+      <c r="T2" s="168"/>
+      <c r="U2" s="169" t="s">
         <v>13</v>
       </c>
-      <c r="V2" s="155"/>
-      <c r="W2" s="186"/>
-      <c r="X2" s="154" t="s">
+      <c r="V2" s="167"/>
+      <c r="W2" s="168"/>
+      <c r="X2" s="169" t="s">
         <v>14</v>
       </c>
-      <c r="Y2" s="155"/>
-      <c r="Z2" s="155"/>
-      <c r="AA2" s="155"/>
-      <c r="AB2" s="155"/>
-      <c r="AC2" s="156"/>
-      <c r="AD2" s="157" t="s">
+      <c r="Y2" s="167"/>
+      <c r="Z2" s="167"/>
+      <c r="AA2" s="167"/>
+      <c r="AB2" s="167"/>
+      <c r="AC2" s="170"/>
+      <c r="AD2" s="171" t="s">
         <v>15</v>
       </c>
-      <c r="AE2" s="158"/>
-      <c r="AF2" s="159"/>
-      <c r="AG2" s="143" t="s">
+      <c r="AE2" s="172"/>
+      <c r="AF2" s="173"/>
+      <c r="AG2" s="174" t="s">
         <v>16</v>
       </c>
-      <c r="AH2" s="144"/>
-      <c r="AI2" s="147"/>
-      <c r="AJ2" s="146" t="s">
+      <c r="AH2" s="175"/>
+      <c r="AI2" s="176"/>
+      <c r="AJ2" s="177" t="s">
         <v>17</v>
       </c>
-      <c r="AK2" s="144"/>
-      <c r="AL2" s="147"/>
-      <c r="AM2" s="144" t="s">
+      <c r="AK2" s="175"/>
+      <c r="AL2" s="176"/>
+      <c r="AM2" s="175" t="s">
         <v>18</v>
       </c>
-      <c r="AN2" s="144"/>
-      <c r="AO2" s="144"/>
-      <c r="AP2" s="146" t="s">
+      <c r="AN2" s="175"/>
+      <c r="AO2" s="175"/>
+      <c r="AP2" s="177" t="s">
         <v>19</v>
       </c>
-      <c r="AQ2" s="144"/>
-      <c r="AR2" s="147"/>
-      <c r="AS2" s="144" t="s">
+      <c r="AQ2" s="175"/>
+      <c r="AR2" s="176"/>
+      <c r="AS2" s="175" t="s">
         <v>20</v>
       </c>
-      <c r="AT2" s="144"/>
-      <c r="AU2" s="144"/>
-      <c r="AV2" s="148" t="s">
+      <c r="AT2" s="175"/>
+      <c r="AU2" s="175"/>
+      <c r="AV2" s="183" t="s">
         <v>21</v>
       </c>
-      <c r="AW2" s="150" t="s">
+      <c r="AW2" s="164" t="s">
         <v>22</v>
       </c>
-      <c r="AX2" s="150" t="s">
+      <c r="AX2" s="164" t="s">
         <v>23</v>
       </c>
-      <c r="AY2" s="152" t="s">
+      <c r="AY2" s="185" t="s">
         <v>24</v>
       </c>
-      <c r="AZ2" s="139" t="s">
+      <c r="AZ2" s="178" t="s">
         <v>25</v>
       </c>
-      <c r="BA2" s="141" t="s">
+      <c r="BA2" s="180" t="s">
         <v>26</v>
       </c>
-      <c r="BB2" s="143" t="s">
+      <c r="BB2" s="174" t="s">
         <v>27</v>
       </c>
-      <c r="BC2" s="144"/>
-      <c r="BD2" s="144"/>
-      <c r="BE2" s="144"/>
-      <c r="BF2" s="145"/>
+      <c r="BC2" s="175"/>
+      <c r="BD2" s="175"/>
+      <c r="BE2" s="175"/>
+      <c r="BF2" s="182"/>
       <c r="BP2" s="6"/>
       <c r="BQ2" s="6"/>
       <c r="BR2" s="6"/>
@@ -3855,14 +3871,14 @@
       <c r="D3" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="E3" s="179"/>
+      <c r="E3" s="158"/>
       <c r="F3" s="11" t="s">
         <v>32</v>
       </c>
       <c r="G3" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="H3" s="181"/>
+      <c r="H3" s="160"/>
       <c r="I3" s="13" t="s">
         <v>34</v>
       </c>
@@ -3878,7 +3894,7 @@
       <c r="M3" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="N3" s="162"/>
+      <c r="N3" s="141"/>
       <c r="O3" s="16" t="s">
         <v>34</v>
       </c>
@@ -3978,12 +3994,12 @@
       <c r="AU3" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="AV3" s="149"/>
-      <c r="AW3" s="151"/>
-      <c r="AX3" s="151"/>
-      <c r="AY3" s="153"/>
-      <c r="AZ3" s="140"/>
-      <c r="BA3" s="142"/>
+      <c r="AV3" s="184"/>
+      <c r="AW3" s="165"/>
+      <c r="AX3" s="165"/>
+      <c r="AY3" s="186"/>
+      <c r="AZ3" s="179"/>
+      <c r="BA3" s="181"/>
       <c r="BB3" s="34" t="s">
         <v>10</v>
       </c>
@@ -6366,6 +6382,19 @@
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="AZ2:AZ3"/>
+    <mergeCell ref="BA2:BA3"/>
+    <mergeCell ref="BB2:BF2"/>
+    <mergeCell ref="AP2:AR2"/>
+    <mergeCell ref="AS2:AU2"/>
+    <mergeCell ref="AV2:AV3"/>
+    <mergeCell ref="AX2:AX3"/>
+    <mergeCell ref="AY2:AY3"/>
+    <mergeCell ref="X2:AC2"/>
+    <mergeCell ref="AD2:AF2"/>
+    <mergeCell ref="AG2:AI2"/>
+    <mergeCell ref="AJ2:AL2"/>
+    <mergeCell ref="AM2:AO2"/>
     <mergeCell ref="BP1:BQ1"/>
     <mergeCell ref="BR1:BS1"/>
     <mergeCell ref="N2:N3"/>
@@ -6382,19 +6411,6 @@
     <mergeCell ref="O2:Q2"/>
     <mergeCell ref="R2:T2"/>
     <mergeCell ref="U2:W2"/>
-    <mergeCell ref="X2:AC2"/>
-    <mergeCell ref="AD2:AF2"/>
-    <mergeCell ref="AG2:AI2"/>
-    <mergeCell ref="AJ2:AL2"/>
-    <mergeCell ref="AM2:AO2"/>
-    <mergeCell ref="AZ2:AZ3"/>
-    <mergeCell ref="BA2:BA3"/>
-    <mergeCell ref="BB2:BF2"/>
-    <mergeCell ref="AP2:AR2"/>
-    <mergeCell ref="AS2:AU2"/>
-    <mergeCell ref="AV2:AV3"/>
-    <mergeCell ref="AX2:AX3"/>
-    <mergeCell ref="AY2:AY3"/>
   </mergeCells>
   <conditionalFormatting sqref="A1:A3">
     <cfRule type="expression" dxfId="119" priority="125">
@@ -8075,8 +8091,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8164,41 +8180,41 @@
         <v>26.5</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" s="75">
+    <row r="3" spans="1:12" s="192" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="188">
         <v>43760</v>
       </c>
-      <c r="B3" s="76">
+      <c r="B3" s="189">
         <v>341.29</v>
       </c>
-      <c r="C3" s="76">
+      <c r="C3" s="189">
         <v>525.44000000000005</v>
       </c>
-      <c r="D3" s="77">
+      <c r="D3" s="190">
         <v>1370</v>
       </c>
-      <c r="E3" s="77">
+      <c r="E3" s="190">
         <v>336</v>
       </c>
-      <c r="F3" s="77">
+      <c r="F3" s="190">
         <v>167</v>
       </c>
-      <c r="G3" s="77">
+      <c r="G3" s="190">
         <v>420</v>
       </c>
-      <c r="H3" s="77">
+      <c r="H3" s="190">
         <v>102</v>
       </c>
-      <c r="I3" s="76">
+      <c r="I3" s="189">
         <v>15</v>
       </c>
-      <c r="J3" s="79">
+      <c r="J3" s="191">
         <v>3.3452999999999999</v>
       </c>
-      <c r="K3" s="76">
+      <c r="K3" s="189">
         <v>129.19999999999999</v>
       </c>
-      <c r="L3" s="76">
+      <c r="L3" s="189">
         <v>26.8</v>
       </c>
     </row>
@@ -8256,41 +8272,41 @@
         <v>62.9</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" s="75">
+    <row r="6" spans="1:12" s="192" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="188">
         <v>43797</v>
       </c>
-      <c r="B6" s="76">
+      <c r="B6" s="189">
         <v>158.43</v>
       </c>
-      <c r="C6" s="76">
+      <c r="C6" s="189">
         <v>236.64</v>
       </c>
-      <c r="D6" s="77">
+      <c r="D6" s="190">
         <v>1370</v>
       </c>
-      <c r="E6" s="77">
+      <c r="E6" s="190">
         <v>484</v>
       </c>
-      <c r="F6" s="77">
+      <c r="F6" s="190">
         <v>349</v>
       </c>
-      <c r="G6" s="77">
+      <c r="G6" s="190">
         <v>734</v>
       </c>
-      <c r="H6" s="77">
+      <c r="H6" s="190">
         <v>198</v>
       </c>
-      <c r="I6" s="76">
+      <c r="I6" s="189">
         <v>31.5</v>
       </c>
-      <c r="J6" s="79">
+      <c r="J6" s="191">
         <v>7.9013</v>
       </c>
-      <c r="K6" s="76">
+      <c r="K6" s="189">
         <v>207.5</v>
       </c>
-      <c r="L6" s="76">
+      <c r="L6" s="189">
         <v>61.8</v>
       </c>
     </row>
@@ -8366,37 +8382,37 @@
         <v>75.8</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A9" s="75">
+    <row r="9" spans="1:12" s="192" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="188">
         <v>43817</v>
       </c>
-      <c r="B9" s="76">
+      <c r="B9" s="189">
         <v>141.29</v>
       </c>
-      <c r="C9" s="76">
+      <c r="C9" s="189">
         <v>232.35</v>
       </c>
-      <c r="D9" s="77">
+      <c r="D9" s="190">
         <v>1340</v>
       </c>
-      <c r="E9" s="77">
+      <c r="E9" s="190">
         <v>510</v>
       </c>
-      <c r="F9" s="77">
+      <c r="F9" s="190">
         <v>363</v>
       </c>
-      <c r="G9" s="78"/>
-      <c r="H9" s="78"/>
-      <c r="I9" s="76">
+      <c r="G9" s="193"/>
+      <c r="H9" s="193"/>
+      <c r="I9" s="189">
         <v>37.5</v>
       </c>
-      <c r="J9" s="79">
+      <c r="J9" s="191">
         <v>6.2276999999999996</v>
       </c>
-      <c r="K9" s="76">
+      <c r="K9" s="189">
         <v>223.9</v>
       </c>
-      <c r="L9" s="76">
+      <c r="L9" s="189">
         <v>73.900000000000006</v>
       </c>
     </row>
@@ -8472,41 +8488,41 @@
         <v>59</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A12" s="75">
+    <row r="12" spans="1:12" s="192" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="188">
         <v>43867</v>
       </c>
-      <c r="B12" s="76">
+      <c r="B12" s="189">
         <v>135.85</v>
       </c>
-      <c r="C12" s="76">
+      <c r="C12" s="189">
         <v>255.71</v>
       </c>
-      <c r="D12" s="77">
+      <c r="D12" s="190">
         <v>1020</v>
       </c>
-      <c r="E12" s="77">
+      <c r="E12" s="190">
         <v>365</v>
       </c>
-      <c r="F12" s="77">
+      <c r="F12" s="190">
         <v>298</v>
       </c>
-      <c r="G12" s="77">
+      <c r="G12" s="190">
         <v>630</v>
       </c>
-      <c r="H12" s="77">
+      <c r="H12" s="190">
         <v>221</v>
       </c>
-      <c r="I12" s="76">
+      <c r="I12" s="189">
         <v>41.9</v>
       </c>
-      <c r="J12" s="79">
+      <c r="J12" s="191">
         <v>6.6729000000000003</v>
       </c>
-      <c r="K12" s="76">
+      <c r="K12" s="189">
         <v>155.4</v>
       </c>
-      <c r="L12" s="76">
+      <c r="L12" s="189">
         <v>60.6</v>
       </c>
     </row>
@@ -8560,6 +8576,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -8570,8 +8587,8 @@
   </sheetPr>
   <dimension ref="A1:X54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="T1" activePane="topRight" state="frozen"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="U18" sqref="U18:U21"/>
     </sheetView>
   </sheetViews>

</xml_diff>